<commit_message>
think thats the last bug fixed
</commit_message>
<xml_diff>
--- a/foo.xlsx
+++ b/foo.xlsx
@@ -73,10 +73,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +373,7 @@
       <c r="B3" s="2">
         <v>44561</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.2488078703703704</v>
       </c>
     </row>

</xml_diff>